<commit_message>
Added updated requisites files from Spring 2026 (1261) term
</commit_message>
<xml_diff>
--- a/Departments/BPK.xlsx
+++ b/Departments/BPK.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mitali\Current project\CourseMaps\CourseMap_Sigma\Departments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpattani\Documents\Course_Requisites\Departments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E755EDC9-9B9C-42C7-9494-E19EB7C1EA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847E0E02-8F5B-4D98-A748-85A76E012C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{22BCF4EB-9D0F-4EBB-9CA3-3E2DDB3E0BCC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{22BCF4EB-9D0F-4EBB-9CA3-3E2DDB3E0BCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$127</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="426">
   <si>
     <t>Course_Code</t>
   </si>
@@ -114,9 +117,6 @@
     <t>BISC100,BISC113,BISCX12,BPK105,BPK110,BPK143,CHEMX12,HSCI100,PHYSX12</t>
   </si>
   <si>
-    <t>REQ-One of Grade 12 Anatomy and Physiology, Biology, Chemistry or Physics with a grade of B or better; or one of BPK 105, BPK 110, BPK 143, BISC 100, BISC 113 or HSCI 100 with a grade of C or better.   Breadth-Science.</t>
-  </si>
-  <si>
     <t>BPK143</t>
   </si>
   <si>
@@ -129,9 +129,6 @@
     <t>BPK 207 - Sensorimotor Control and Learning</t>
   </si>
   <si>
-    <t>REQ-   BPK 142 or permission of instructor.</t>
-  </si>
-  <si>
     <t>BPK208</t>
   </si>
   <si>
@@ -183,18 +180,12 @@
     <t>MATHEMATIC</t>
   </si>
   <si>
-    <t>REQ-Pre-Calculus 12 (or equiv) with a grade of at least A, or MATH 100 grade of at least B, or satisfactory grade on the SFU Calculus Readiness Test. Students with credit for either MATH 150,154 or 157 may not take MATH 151 for further credit.</t>
-  </si>
-  <si>
     <t>MATH152</t>
   </si>
   <si>
     <t>MATH 152 - Calculus II</t>
   </si>
   <si>
-    <t>FANX99,MATH150,MATH151,MATH154,MATH155,MATH157</t>
-  </si>
-  <si>
     <t>REQ-MATH 150 or 151 or 155, with a minimum grade of C-; or MATH 154 or 157, with a grade of at least B. Students with credit for MATH 158 or 251 may not take this course for further credit. Quantitative.</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>FANX99,PHYS125</t>
   </si>
   <si>
-    <t>Prerequisite: PHYS 125 with a minimum grade of C- or permission of the department. Corequisite: MATH 152. Recommended Corequisite: PHYS 133.  Students with credit in PHYS 102, 121 or 141 may not take this course for further credit. Quantitative.</t>
-  </si>
-  <si>
     <t>PHYS141</t>
   </si>
   <si>
@@ -318,9 +306,6 @@
     <t>BPK 305 - Human Physiology I</t>
   </si>
   <si>
-    <t>BPK205,MATH155</t>
-  </si>
-  <si>
     <t>REQ-BPK 205, MBB 231 (or 201), MATH 155 (or 152). Majors from outside BPK require BPK 205 (or BISC 305), MBB 231 (or 201), MATH 155 (or 152) plus permission of the instructor.</t>
   </si>
   <si>
@@ -420,9 +405,6 @@
     <t>BPK 401 - Muscle Biomechanics</t>
   </si>
   <si>
-    <t>BPK201,BPK205,BPK208</t>
-  </si>
-  <si>
     <t>REQ-90 credits, BPK 201 and 205, or BPK 208.  Students with credit for BPK 421, Muscle Biomechanics, may not take this course for further credit.</t>
   </si>
   <si>
@@ -627,36 +609,9 @@
     <t>BPK 812 - Molecular and Cellular Cardiology</t>
   </si>
   <si>
-    <t>BPK831</t>
-  </si>
-  <si>
-    <t>BPK 831 - Current Topics in Thermophysiology</t>
-  </si>
-  <si>
-    <t>BPK840</t>
-  </si>
-  <si>
-    <t>BPK 840 - Human Biomechanics</t>
-  </si>
-  <si>
-    <t>BPK851</t>
-  </si>
-  <si>
-    <t>BPK 851 - Recent Advances in Experimental Carcinogenesis</t>
-  </si>
-  <si>
     <t>BPK431</t>
   </si>
   <si>
-    <t>REQ: BPK (or KIN) 431.</t>
-  </si>
-  <si>
-    <t>BPK870</t>
-  </si>
-  <si>
-    <t>BPK 870 - Experiments and Models in Physiology</t>
-  </si>
-  <si>
     <t>BPK895</t>
   </si>
   <si>
@@ -705,9 +660,6 @@
     <t>MBB 231 - Cellular Biology and Biochemistry</t>
   </si>
   <si>
-    <t>BISC101,CHEM281,CHEM282,CHEM283,MBB222</t>
-  </si>
-  <si>
     <t>CHEM282,CHEM283</t>
   </si>
   <si>
@@ -840,9 +792,6 @@
     <t>BPK142,FANX99,MATH150,MATH151,MATH152,MATH154,MATH155,PHYS101,PHYS120,PHYS125,PHYS140</t>
   </si>
   <si>
-    <t>REQ- MATH 150, 151 or 154, MATH 152 or 155 (may be taken concurrently), PHYS 101 (or 120 or 125 or 140), BPK 142.</t>
-  </si>
-  <si>
     <t>BPK205</t>
   </si>
   <si>
@@ -954,18 +903,12 @@
     <t>MATH 150 - Calculus I with Review</t>
   </si>
   <si>
-    <t>REQ-Pre-Calc 12 (or eqv.) with at least B+, or MATH100 with at least B-, or achieving satisfactory grade on SFU Calculus Readiness Test. Students with credit for either MATH151,154 or 157 may not take MATH150 for further credit. Quantitative.</t>
-  </si>
-  <si>
     <t>MATH154</t>
   </si>
   <si>
     <t>MATH 154 - Mathematics for the Life Sciences I</t>
   </si>
   <si>
-    <t>REQ-Pre-Calc 12 (or equiv.) with at least B, or MATH 100 with at least C-, or achieving a satis. grade on the SFU Calculus Readiness Test. Students with cred. for MATH 150, 151 or 157 may not take MATH 154 for further credit. Quantitative</t>
-  </si>
-  <si>
     <t>MATH155</t>
   </si>
   <si>
@@ -987,9 +930,6 @@
     <t>MBB331</t>
   </si>
   <si>
-    <t>REQ or corequisite: MBB 331 with a minimum grade of C-.  Students with credit for BISC 357 may not take this course for further credit.</t>
-  </si>
-  <si>
     <t>PHYS101</t>
   </si>
   <si>
@@ -1233,9 +1173,6 @@
     <t>BPK352,FALX99</t>
   </si>
   <si>
-    <t>REQ-BPK 352.</t>
-  </si>
-  <si>
     <t>BPK 457 - Behavioural Neuroscience Undergraduate Honours Thesis Proposal</t>
   </si>
   <si>
@@ -1342,6 +1279,45 @@
   </si>
   <si>
     <t>CoRequisites</t>
+  </si>
+  <si>
+    <t>REQ-One of Grade 12 Anatomy and Physiology, Biology, Chemistry or Physics with a grade of B or better; or one of BPK 105, BPK 110, BPK 143, BISC 100, BISC 113 or HSCI 100 with a grade of C or better. Breadth-Science.</t>
+  </si>
+  <si>
+    <t>REQ- MATH 150, 151 or 154; MATH 152 or 155 (may be taken concurrently); PHYS 101 (or 120 or 125 or 140); BPK 142. Quantitative</t>
+  </si>
+  <si>
+    <t>REQ-BPK 142.</t>
+  </si>
+  <si>
+    <t>BPK205,MATH152,MATH155</t>
+  </si>
+  <si>
+    <t>REQ-BPK 352. Writing</t>
+  </si>
+  <si>
+    <t>REQ-Pre-Calculus 12 (or equivalent) with a grade of at least B+, or MATH 100 with a grade of at least B-.  Students with credit for either MATH 151, 154 or 157 may not take MATH 150 for further credit. Quantitative.</t>
+  </si>
+  <si>
+    <t>REQ- Pre-Calculus 12 (or equivalent) with a grade of at least A, or MATH 100 with a grade of at least B.  Students with credit for either MATH 150, 154 or 157 may not take MATH 151 for further credit. Quantitative.</t>
+  </si>
+  <si>
+    <t>FANX99,MATH100,MATH110,MATHX12</t>
+  </si>
+  <si>
+    <t>REQ-Pre-Calculus 12 (or equivalent) with a grade of at least B, or MATH 100 with a grade of at least C-, or MATH 110 with a grade of at least C-. Students with credit for either MATH 150, 151 or 157 may not take MATH 154 for further credit. Quantitative.</t>
+  </si>
+  <si>
+    <t>BISC101,CHEM281,MBB222</t>
+  </si>
+  <si>
+    <t>MBB229</t>
+  </si>
+  <si>
+    <t>REQ-MBB 229 with a minimum grade of C. Corequisite: MBB 331. Students with credit for BISC 357 may not take this course for further credit.</t>
+  </si>
+  <si>
+    <t>REQ-PHYS 125 with a minimum grade of C- or permission of the department. Corequisite: MATH 152. Recommended Corequisite: PHYS 133. Students with credit in PHYS 102, 121 or 141 may not take this course for further credit. Quantitative.</t>
   </si>
 </sst>
 </file>
@@ -1696,7 +1672,7 @@
   <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="A2" sqref="A2:I123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1715,10 +1691,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>433</v>
+        <v>411</v>
       </c>
       <c r="F1" t="s">
-        <v>434</v>
+        <v>412</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1732,42 +1708,45 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>226</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -1779,24 +1758,24 @@
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>229</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>230</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -1805,24 +1784,27 @@
         <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>232</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>233</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -1831,27 +1813,24 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -1860,24 +1839,27 @@
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>71</v>
+      </c>
+      <c r="I6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -1886,56 +1868,56 @@
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>234</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>235</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>236</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -1944,27 +1926,24 @@
         <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -1973,27 +1952,24 @@
         <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>275</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>276</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>277</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
@@ -2002,27 +1978,27 @@
         <v>18</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s">
-        <v>48</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>237</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>238</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -2031,15 +2007,12 @@
         <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>239</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -2048,7 +2021,7 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>240</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -2061,113 +2034,104 @@
       </c>
       <c r="H13" t="s">
         <v>19</v>
-      </c>
-      <c r="I13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I14" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
         <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
         <v>18</v>
       </c>
       <c r="H16" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -2176,21 +2140,21 @@
         <v>18</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>241</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>242</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -2202,24 +2166,24 @@
         <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>243</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>244</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>245</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -2228,56 +2192,56 @@
         <v>18</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>247</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>248</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>249</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
         <v>18</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>86</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>250</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>251</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>252</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -2286,15 +2250,15 @@
         <v>18</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>90</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -2303,10 +2267,10 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
@@ -2318,12 +2282,12 @@
         <v>19</v>
       </c>
       <c r="I22" t="s">
-        <v>94</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -2332,13 +2296,13 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
         <v>18</v>
@@ -2347,12 +2311,12 @@
         <v>19</v>
       </c>
       <c r="I23" t="s">
-        <v>98</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>254</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -2361,10 +2325,10 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>255</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -2374,14 +2338,11 @@
       </c>
       <c r="H24" t="s">
         <v>19</v>
-      </c>
-      <c r="I24" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>256</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -2390,10 +2351,10 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>104</v>
+        <v>257</v>
       </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
@@ -2405,12 +2366,12 @@
         <v>19</v>
       </c>
       <c r="I25" t="s">
-        <v>106</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -2419,10 +2380,10 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
         <v>12</v>
@@ -2434,12 +2395,12 @@
         <v>19</v>
       </c>
       <c r="I26" t="s">
-        <v>110</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>259</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -2448,10 +2409,10 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="E27" t="s">
-        <v>113</v>
+        <v>261</v>
       </c>
       <c r="F27" t="s">
         <v>12</v>
@@ -2463,12 +2424,12 @@
         <v>19</v>
       </c>
       <c r="I27" t="s">
-        <v>114</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -2477,10 +2438,10 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
@@ -2492,12 +2453,12 @@
         <v>19</v>
       </c>
       <c r="I28" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -2506,10 +2467,10 @@
         <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="E29" t="s">
-        <v>22</v>
+        <v>416</v>
       </c>
       <c r="F29" t="s">
         <v>12</v>
@@ -2521,12 +2482,12 @@
         <v>19</v>
       </c>
       <c r="I29" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -2535,13 +2496,13 @@
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>263</v>
       </c>
       <c r="E30" t="s">
-        <v>119</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="G30" t="s">
         <v>18</v>
@@ -2550,12 +2511,12 @@
         <v>19</v>
       </c>
       <c r="I30" t="s">
-        <v>124</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -2564,13 +2525,13 @@
         <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="E31" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="G31" t="s">
         <v>18</v>
@@ -2579,12 +2540,12 @@
         <v>19</v>
       </c>
       <c r="I31" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -2593,10 +2554,10 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
@@ -2608,12 +2569,12 @@
         <v>19</v>
       </c>
       <c r="I32" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
@@ -2622,10 +2583,10 @@
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="F33" t="s">
         <v>12</v>
@@ -2637,12 +2598,12 @@
         <v>19</v>
       </c>
       <c r="I33" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -2651,10 +2612,10 @@
         <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="E34" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
@@ -2666,12 +2627,12 @@
         <v>19</v>
       </c>
       <c r="I34" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>265</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -2680,10 +2641,10 @@
         <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>266</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
+        <v>103</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -2695,12 +2656,12 @@
         <v>19</v>
       </c>
       <c r="I35" t="s">
-        <v>144</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>268</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
@@ -2709,10 +2670,10 @@
         <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>146</v>
+        <v>269</v>
       </c>
       <c r="E36" t="s">
-        <v>147</v>
+        <v>270</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
@@ -2724,12 +2685,12 @@
         <v>19</v>
       </c>
       <c r="I36" t="s">
-        <v>148</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>272</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
@@ -2738,7 +2699,7 @@
         <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>150</v>
+        <v>273</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -2751,11 +2712,14 @@
       </c>
       <c r="H37" t="s">
         <v>19</v>
+      </c>
+      <c r="I37" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
@@ -2764,10 +2728,10 @@
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
@@ -2777,11 +2741,14 @@
       </c>
       <c r="H38" t="s">
         <v>19</v>
+      </c>
+      <c r="I38" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -2790,10 +2757,10 @@
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="E39" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="F39" t="s">
         <v>12</v>
@@ -2805,12 +2772,12 @@
         <v>19</v>
       </c>
       <c r="I39" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>157</v>
+        <v>315</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -2819,13 +2786,13 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>158</v>
+        <v>316</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
+        <v>317</v>
       </c>
       <c r="F40" t="s">
-        <v>159</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
         <v>18</v>
@@ -2834,12 +2801,12 @@
         <v>19</v>
       </c>
       <c r="I40" t="s">
-        <v>160</v>
+        <v>318</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>161</v>
+        <v>319</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -2848,13 +2815,13 @@
         <v>16</v>
       </c>
       <c r="D41" t="s">
-        <v>162</v>
+        <v>320</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>321</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="G41" t="s">
         <v>18</v>
@@ -2863,12 +2830,12 @@
         <v>19</v>
       </c>
       <c r="I41" t="s">
-        <v>163</v>
+        <v>322</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -2877,10 +2844,10 @@
         <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
       <c r="E42" t="s">
-        <v>122</v>
+        <v>22</v>
       </c>
       <c r="F42" t="s">
         <v>12</v>
@@ -2892,12 +2859,12 @@
         <v>19</v>
       </c>
       <c r="I42" t="s">
-        <v>166</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -2906,10 +2873,10 @@
         <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="E43" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="F43" t="s">
         <v>12</v>
@@ -2921,12 +2888,12 @@
         <v>19</v>
       </c>
       <c r="I43" t="s">
-        <v>169</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>170</v>
+        <v>323</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -2935,10 +2902,10 @@
         <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>171</v>
+        <v>324</v>
       </c>
       <c r="E44" t="s">
-        <v>167</v>
+        <v>270</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
@@ -2950,12 +2917,12 @@
         <v>19</v>
       </c>
       <c r="I44" t="s">
-        <v>172</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>173</v>
+        <v>326</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
@@ -2964,13 +2931,13 @@
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>174</v>
+        <v>327</v>
       </c>
       <c r="E45" t="s">
-        <v>175</v>
+        <v>328</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="G45" t="s">
         <v>18</v>
@@ -2979,12 +2946,12 @@
         <v>19</v>
       </c>
       <c r="I45" t="s">
-        <v>176</v>
+        <v>329</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
@@ -2993,13 +2960,13 @@
         <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="E46" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F46" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G46" t="s">
         <v>18</v>
@@ -3008,12 +2975,12 @@
         <v>19</v>
       </c>
       <c r="I46" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>122</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -3022,13 +2989,13 @@
         <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
       <c r="E47" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="F47" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
         <v>18</v>
@@ -3037,12 +3004,12 @@
         <v>19</v>
       </c>
       <c r="I47" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>184</v>
+        <v>330</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
@@ -3051,13 +3018,13 @@
         <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>185</v>
+        <v>331</v>
       </c>
       <c r="E48" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="F48" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s">
         <v>18</v>
@@ -3066,12 +3033,12 @@
         <v>19</v>
       </c>
       <c r="I48" t="s">
-        <v>187</v>
+        <v>332</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>188</v>
+        <v>126</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
@@ -3080,10 +3047,10 @@
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>189</v>
+        <v>127</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="F49" t="s">
         <v>12</v>
@@ -3093,11 +3060,14 @@
       </c>
       <c r="H49" t="s">
         <v>19</v>
+      </c>
+      <c r="I49" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
@@ -3106,10 +3076,10 @@
         <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>191</v>
+        <v>131</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="F50" t="s">
         <v>12</v>
@@ -3119,11 +3089,14 @@
       </c>
       <c r="H50" t="s">
         <v>19</v>
+      </c>
+      <c r="I50" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>192</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
@@ -3132,10 +3105,10 @@
         <v>16</v>
       </c>
       <c r="D51" t="s">
-        <v>193</v>
+        <v>135</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="F51" t="s">
         <v>12</v>
@@ -3145,11 +3118,14 @@
       </c>
       <c r="H51" t="s">
         <v>19</v>
+      </c>
+      <c r="I51" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
@@ -3158,10 +3134,10 @@
         <v>16</v>
       </c>
       <c r="D52" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="E52" t="s">
-        <v>12</v>
+        <v>140</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
@@ -3171,11 +3147,14 @@
       </c>
       <c r="H52" t="s">
         <v>19</v>
+      </c>
+      <c r="I52" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>196</v>
+        <v>333</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
@@ -3184,10 +3163,10 @@
         <v>16</v>
       </c>
       <c r="D53" t="s">
-        <v>197</v>
+        <v>334</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="F53" t="s">
         <v>12</v>
@@ -3197,11 +3176,14 @@
       </c>
       <c r="H53" t="s">
         <v>19</v>
+      </c>
+      <c r="I53" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>336</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
@@ -3210,10 +3192,10 @@
         <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>199</v>
+        <v>337</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>338</v>
       </c>
       <c r="F54" t="s">
         <v>12</v>
@@ -3223,11 +3205,14 @@
       </c>
       <c r="H54" t="s">
         <v>19</v>
+      </c>
+      <c r="I54" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>200</v>
+        <v>340</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -3236,10 +3221,10 @@
         <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>201</v>
+        <v>341</v>
       </c>
       <c r="E55" t="s">
-        <v>202</v>
+        <v>342</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
@@ -3251,12 +3236,12 @@
         <v>19</v>
       </c>
       <c r="I55" t="s">
-        <v>203</v>
+        <v>343</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>204</v>
+        <v>344</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -3265,10 +3250,10 @@
         <v>16</v>
       </c>
       <c r="D56" t="s">
-        <v>205</v>
+        <v>345</v>
       </c>
       <c r="E56" t="s">
-        <v>12</v>
+        <v>346</v>
       </c>
       <c r="F56" t="s">
         <v>12</v>
@@ -3282,7 +3267,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>206</v>
+        <v>142</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
@@ -3291,7 +3276,7 @@
         <v>16</v>
       </c>
       <c r="D57" t="s">
-        <v>207</v>
+        <v>143</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -3308,7 +3293,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>208</v>
+        <v>347</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -3317,7 +3302,7 @@
         <v>16</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
+        <v>348</v>
       </c>
       <c r="E58" t="s">
         <v>12</v>
@@ -3334,16 +3319,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>210</v>
+        <v>349</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D59" t="s">
-        <v>211</v>
+        <v>350</v>
       </c>
       <c r="E59" t="s">
         <v>12</v>
@@ -3355,21 +3340,21 @@
         <v>18</v>
       </c>
       <c r="H59" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>210</v>
+        <v>144</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D60" t="s">
-        <v>211</v>
+        <v>145</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
@@ -3381,82 +3366,82 @@
         <v>18</v>
       </c>
       <c r="H60" t="s">
-        <v>47</v>
-      </c>
-      <c r="I60" t="s">
-        <v>212</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>213</v>
+        <v>351</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="D61" t="s">
-        <v>215</v>
+        <v>352</v>
       </c>
       <c r="E61" t="s">
-        <v>216</v>
+        <v>353</v>
       </c>
       <c r="F61" t="s">
-        <v>217</v>
+        <v>91</v>
       </c>
       <c r="G61" t="s">
         <v>18</v>
       </c>
       <c r="H61" t="s">
-        <v>218</v>
+        <v>19</v>
       </c>
       <c r="I61" t="s">
-        <v>219</v>
+        <v>354</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>221</v>
+        <v>355</v>
       </c>
       <c r="E62" t="s">
-        <v>222</v>
+        <v>356</v>
       </c>
       <c r="F62" t="s">
-        <v>223</v>
+        <v>12</v>
       </c>
       <c r="G62" t="s">
         <v>18</v>
       </c>
       <c r="H62" t="s">
-        <v>218</v>
+        <v>19</v>
+      </c>
+      <c r="I62" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>224</v>
+        <v>358</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>225</v>
+        <v>16</v>
       </c>
       <c r="D63" t="s">
-        <v>226</v>
+        <v>359</v>
       </c>
       <c r="E63" t="s">
-        <v>210</v>
+        <v>360</v>
       </c>
       <c r="F63" t="s">
         <v>12</v>
@@ -3465,108 +3450,114 @@
         <v>18</v>
       </c>
       <c r="H63" t="s">
-        <v>227</v>
+        <v>19</v>
       </c>
       <c r="I63" t="s">
-        <v>228</v>
+        <v>361</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>229</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D64" t="s">
-        <v>230</v>
+        <v>151</v>
       </c>
       <c r="E64" t="s">
-        <v>231</v>
+        <v>152</v>
       </c>
       <c r="F64" t="s">
-        <v>232</v>
+        <v>152</v>
       </c>
       <c r="G64" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H64" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I64" t="s">
-        <v>233</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>234</v>
+        <v>154</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>235</v>
+        <v>16</v>
       </c>
       <c r="D65" t="s">
-        <v>236</v>
+        <v>155</v>
       </c>
       <c r="E65" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>235</v>
+        <v>18</v>
       </c>
       <c r="H65" t="s">
-        <v>237</v>
+        <v>19</v>
+      </c>
+      <c r="I65" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>238</v>
+        <v>362</v>
       </c>
       <c r="B66" t="s">
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>239</v>
+        <v>16</v>
       </c>
       <c r="D66" t="s">
-        <v>240</v>
+        <v>363</v>
       </c>
       <c r="E66" t="s">
-        <v>12</v>
+        <v>154</v>
       </c>
       <c r="F66" t="s">
         <v>12</v>
       </c>
       <c r="G66" t="s">
-        <v>241</v>
+        <v>18</v>
       </c>
       <c r="H66" t="s">
-        <v>242</v>
+        <v>19</v>
+      </c>
+      <c r="I66" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>365</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D67" t="s">
-        <v>243</v>
+        <v>366</v>
       </c>
       <c r="E67" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="F67" t="s">
         <v>12</v>
@@ -3575,27 +3566,27 @@
         <v>18</v>
       </c>
       <c r="H67" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="I67" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>245</v>
+        <v>368</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D68" t="s">
-        <v>246</v>
+        <v>369</v>
       </c>
       <c r="E68" t="s">
-        <v>247</v>
+        <v>342</v>
       </c>
       <c r="F68" t="s">
         <v>12</v>
@@ -3604,27 +3595,24 @@
         <v>18</v>
       </c>
       <c r="H68" t="s">
-        <v>76</v>
-      </c>
-      <c r="I68" t="s">
-        <v>248</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>249</v>
+        <v>370</v>
       </c>
       <c r="B69" t="s">
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D69" t="s">
-        <v>250</v>
+        <v>371</v>
       </c>
       <c r="E69" t="s">
-        <v>12</v>
+        <v>372</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>
@@ -3633,24 +3621,27 @@
         <v>18</v>
       </c>
       <c r="H69" t="s">
-        <v>76</v>
+        <v>19</v>
+      </c>
+      <c r="I69" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>251</v>
+        <v>157</v>
       </c>
       <c r="B70" t="s">
         <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D70" t="s">
-        <v>252</v>
+        <v>158</v>
       </c>
       <c r="E70" t="s">
-        <v>253</v>
+        <v>116</v>
       </c>
       <c r="F70" t="s">
         <v>12</v>
@@ -3659,12 +3650,15 @@
         <v>18</v>
       </c>
       <c r="H70" t="s">
-        <v>76</v>
+        <v>19</v>
+      </c>
+      <c r="I70" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>254</v>
+        <v>374</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
@@ -3673,10 +3667,10 @@
         <v>16</v>
       </c>
       <c r="D71" t="s">
-        <v>255</v>
+        <v>375</v>
       </c>
       <c r="E71" t="s">
-        <v>12</v>
+        <v>376</v>
       </c>
       <c r="F71" t="s">
         <v>12</v>
@@ -3686,11 +3680,14 @@
       </c>
       <c r="H71" t="s">
         <v>19</v>
+      </c>
+      <c r="I71" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>256</v>
+        <v>160</v>
       </c>
       <c r="B72" t="s">
         <v>8</v>
@@ -3699,10 +3696,10 @@
         <v>16</v>
       </c>
       <c r="D72" t="s">
-        <v>257</v>
+        <v>161</v>
       </c>
       <c r="E72" t="s">
-        <v>12</v>
+        <v>157</v>
       </c>
       <c r="F72" t="s">
         <v>12</v>
@@ -3712,11 +3709,14 @@
       </c>
       <c r="H72" t="s">
         <v>19</v>
+      </c>
+      <c r="I72" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>258</v>
+        <v>163</v>
       </c>
       <c r="B73" t="s">
         <v>8</v>
@@ -3725,10 +3725,10 @@
         <v>16</v>
       </c>
       <c r="D73" t="s">
-        <v>259</v>
+        <v>164</v>
       </c>
       <c r="E73" t="s">
-        <v>12</v>
+        <v>160</v>
       </c>
       <c r="F73" t="s">
         <v>12</v>
@@ -3738,11 +3738,14 @@
       </c>
       <c r="H73" t="s">
         <v>19</v>
+      </c>
+      <c r="I73" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>260</v>
+        <v>168</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
@@ -3751,10 +3754,10 @@
         <v>16</v>
       </c>
       <c r="D74" t="s">
-        <v>261</v>
+        <v>377</v>
       </c>
       <c r="E74" t="s">
-        <v>262</v>
+        <v>378</v>
       </c>
       <c r="F74" t="s">
         <v>12</v>
@@ -3766,12 +3769,12 @@
         <v>19</v>
       </c>
       <c r="I74" t="s">
-        <v>263</v>
+        <v>379</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>264</v>
+        <v>166</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
@@ -3780,13 +3783,13 @@
         <v>16</v>
       </c>
       <c r="D75" t="s">
-        <v>265</v>
+        <v>167</v>
       </c>
       <c r="E75" t="s">
-        <v>266</v>
+        <v>168</v>
       </c>
       <c r="F75" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="G75" t="s">
         <v>18</v>
@@ -3795,12 +3798,12 @@
         <v>19</v>
       </c>
       <c r="I75" t="s">
-        <v>267</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>268</v>
+        <v>380</v>
       </c>
       <c r="B76" t="s">
         <v>8</v>
@@ -3809,10 +3812,10 @@
         <v>16</v>
       </c>
       <c r="D76" t="s">
-        <v>269</v>
+        <v>381</v>
       </c>
       <c r="E76" t="s">
-        <v>270</v>
+        <v>382</v>
       </c>
       <c r="F76" t="s">
         <v>12</v>
@@ -3824,12 +3827,12 @@
         <v>19</v>
       </c>
       <c r="I76" t="s">
-        <v>271</v>
+        <v>383</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>272</v>
+        <v>384</v>
       </c>
       <c r="B77" t="s">
         <v>8</v>
@@ -3838,24 +3841,27 @@
         <v>16</v>
       </c>
       <c r="D77" t="s">
-        <v>273</v>
+        <v>385</v>
       </c>
       <c r="E77" t="s">
-        <v>12</v>
+        <v>386</v>
       </c>
       <c r="F77" t="s">
-        <v>12</v>
+        <v>380</v>
       </c>
       <c r="G77" t="s">
         <v>18</v>
       </c>
       <c r="H77" t="s">
         <v>19</v>
+      </c>
+      <c r="I77" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>274</v>
+        <v>146</v>
       </c>
       <c r="B78" t="s">
         <v>8</v>
@@ -3864,10 +3870,10 @@
         <v>16</v>
       </c>
       <c r="D78" t="s">
-        <v>275</v>
+        <v>147</v>
       </c>
       <c r="E78" t="s">
-        <v>22</v>
+        <v>148</v>
       </c>
       <c r="F78" t="s">
         <v>12</v>
@@ -3879,12 +3885,12 @@
         <v>19</v>
       </c>
       <c r="I78" t="s">
-        <v>276</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>277</v>
+        <v>170</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
@@ -3893,13 +3899,13 @@
         <v>16</v>
       </c>
       <c r="D79" t="s">
-        <v>278</v>
+        <v>171</v>
       </c>
       <c r="E79" t="s">
-        <v>279</v>
+        <v>37</v>
       </c>
       <c r="F79" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G79" t="s">
         <v>18</v>
@@ -3908,12 +3914,12 @@
         <v>19</v>
       </c>
       <c r="I79" t="s">
-        <v>280</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>179</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
@@ -3922,13 +3928,13 @@
         <v>16</v>
       </c>
       <c r="D80" t="s">
-        <v>281</v>
+        <v>388</v>
       </c>
       <c r="E80" t="s">
-        <v>28</v>
+        <v>170</v>
       </c>
       <c r="F80" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="G80" t="s">
         <v>18</v>
@@ -3937,12 +3943,12 @@
         <v>19</v>
       </c>
       <c r="I80" t="s">
-        <v>282</v>
+        <v>389</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>283</v>
+        <v>173</v>
       </c>
       <c r="B81" t="s">
         <v>8</v>
@@ -3951,13 +3957,13 @@
         <v>16</v>
       </c>
       <c r="D81" t="s">
-        <v>284</v>
+        <v>174</v>
       </c>
       <c r="E81" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
       <c r="F81" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G81" t="s">
         <v>18</v>
@@ -3966,12 +3972,12 @@
         <v>19</v>
       </c>
       <c r="I81" t="s">
-        <v>285</v>
+        <v>176</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>286</v>
+        <v>390</v>
       </c>
       <c r="B82" t="s">
         <v>8</v>
@@ -3980,13 +3986,13 @@
         <v>16</v>
       </c>
       <c r="D82" t="s">
-        <v>287</v>
+        <v>391</v>
       </c>
       <c r="E82" t="s">
-        <v>288</v>
+        <v>175</v>
       </c>
       <c r="F82" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G82" t="s">
         <v>18</v>
@@ -3995,12 +4001,12 @@
         <v>19</v>
       </c>
       <c r="I82" t="s">
-        <v>289</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>290</v>
+        <v>177</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
@@ -4009,13 +4015,13 @@
         <v>16</v>
       </c>
       <c r="D83" t="s">
-        <v>291</v>
+        <v>178</v>
       </c>
       <c r="E83" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="F83" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
       <c r="G83" t="s">
         <v>18</v>
@@ -4024,24 +4030,24 @@
         <v>19</v>
       </c>
       <c r="I83" t="s">
-        <v>292</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>293</v>
+        <v>181</v>
       </c>
       <c r="B84" t="s">
         <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D84" t="s">
-        <v>294</v>
+        <v>182</v>
       </c>
       <c r="E84" t="s">
-        <v>295</v>
+        <v>12</v>
       </c>
       <c r="F84" t="s">
         <v>12</v>
@@ -4050,56 +4056,50 @@
         <v>18</v>
       </c>
       <c r="H84" t="s">
-        <v>76</v>
-      </c>
-      <c r="I84" t="s">
-        <v>296</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>217</v>
+        <v>392</v>
       </c>
       <c r="B85" t="s">
         <v>8</v>
       </c>
       <c r="C85" t="s">
-        <v>297</v>
+        <v>16</v>
       </c>
       <c r="D85" t="s">
-        <v>298</v>
+        <v>393</v>
       </c>
       <c r="E85" t="s">
-        <v>299</v>
+        <v>12</v>
       </c>
       <c r="F85" t="s">
-        <v>300</v>
+        <v>12</v>
       </c>
       <c r="G85" t="s">
         <v>18</v>
       </c>
       <c r="H85" t="s">
-        <v>301</v>
-      </c>
-      <c r="I85" t="s">
-        <v>302</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>303</v>
+        <v>394</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
       </c>
       <c r="C86" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D86" t="s">
-        <v>304</v>
+        <v>395</v>
       </c>
       <c r="E86" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="F86" t="s">
         <v>12</v>
@@ -4108,27 +4108,24 @@
         <v>18</v>
       </c>
       <c r="H86" t="s">
-        <v>47</v>
-      </c>
-      <c r="I86" t="s">
-        <v>305</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>306</v>
+        <v>183</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D87" t="s">
-        <v>307</v>
+        <v>184</v>
       </c>
       <c r="E87" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="F87" t="s">
         <v>12</v>
@@ -4137,27 +4134,24 @@
         <v>18</v>
       </c>
       <c r="H87" t="s">
-        <v>47</v>
-      </c>
-      <c r="I87" t="s">
-        <v>308</v>
+        <v>19</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>309</v>
+        <v>185</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D88" t="s">
-        <v>310</v>
+        <v>186</v>
       </c>
       <c r="E88" t="s">
-        <v>311</v>
+        <v>12</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
@@ -4166,189 +4160,168 @@
         <v>18</v>
       </c>
       <c r="H88" t="s">
-        <v>47</v>
-      </c>
-      <c r="I88" t="s">
-        <v>312</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>313</v>
+        <v>396</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>214</v>
+        <v>16</v>
       </c>
       <c r="D89" t="s">
-        <v>314</v>
+        <v>397</v>
       </c>
       <c r="E89" t="s">
-        <v>315</v>
+        <v>12</v>
       </c>
       <c r="F89" t="s">
-        <v>315</v>
+        <v>12</v>
       </c>
       <c r="G89" t="s">
         <v>18</v>
       </c>
       <c r="H89" t="s">
-        <v>218</v>
-      </c>
-      <c r="I89" t="s">
-        <v>316</v>
+        <v>19</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>317</v>
+        <v>187</v>
       </c>
       <c r="B90" t="s">
         <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D90" t="s">
-        <v>318</v>
+        <v>188</v>
       </c>
       <c r="E90" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="F90" t="s">
-        <v>319</v>
+        <v>12</v>
       </c>
       <c r="G90" t="s">
         <v>18</v>
       </c>
       <c r="H90" t="s">
-        <v>61</v>
-      </c>
-      <c r="I90" t="s">
-        <v>320</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>321</v>
+        <v>190</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
       </c>
       <c r="C91" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D91" t="s">
-        <v>322</v>
+        <v>191</v>
       </c>
       <c r="E91" t="s">
-        <v>323</v>
+        <v>12</v>
       </c>
       <c r="F91" t="s">
-        <v>324</v>
+        <v>12</v>
       </c>
       <c r="G91" t="s">
         <v>18</v>
       </c>
       <c r="H91" t="s">
-        <v>61</v>
-      </c>
-      <c r="I91" t="s">
-        <v>325</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>326</v>
+        <v>192</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
       </c>
       <c r="C92" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D92" t="s">
-        <v>327</v>
+        <v>193</v>
       </c>
       <c r="E92" t="s">
-        <v>328</v>
+        <v>12</v>
       </c>
       <c r="F92" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="G92" t="s">
         <v>18</v>
       </c>
       <c r="H92" t="s">
-        <v>61</v>
-      </c>
-      <c r="I92" t="s">
-        <v>329</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>330</v>
+        <v>398</v>
       </c>
       <c r="B93" t="s">
         <v>8</v>
       </c>
       <c r="C93" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D93" t="s">
-        <v>331</v>
+        <v>399</v>
       </c>
       <c r="E93" t="s">
-        <v>210</v>
+        <v>12</v>
       </c>
       <c r="F93" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="G93" t="s">
         <v>18</v>
       </c>
       <c r="H93" t="s">
-        <v>61</v>
-      </c>
-      <c r="I93" t="s">
-        <v>332</v>
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>333</v>
+        <v>400</v>
       </c>
       <c r="B94" t="s">
         <v>8</v>
       </c>
       <c r="C94" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D94" t="s">
-        <v>334</v>
+        <v>401</v>
       </c>
       <c r="E94" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="F94" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="G94" t="s">
         <v>18</v>
       </c>
       <c r="H94" t="s">
-        <v>61</v>
-      </c>
-      <c r="I94" t="s">
-        <v>335</v>
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>336</v>
+        <v>402</v>
       </c>
       <c r="B95" t="s">
         <v>8</v>
@@ -4357,10 +4330,10 @@
         <v>16</v>
       </c>
       <c r="D95" t="s">
-        <v>337</v>
+        <v>403</v>
       </c>
       <c r="E95" t="s">
-        <v>338</v>
+        <v>12</v>
       </c>
       <c r="F95" t="s">
         <v>12</v>
@@ -4370,14 +4343,11 @@
       </c>
       <c r="H95" t="s">
         <v>19</v>
-      </c>
-      <c r="I95" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>340</v>
+        <v>407</v>
       </c>
       <c r="B96" t="s">
         <v>8</v>
@@ -4386,27 +4356,24 @@
         <v>16</v>
       </c>
       <c r="D96" t="s">
-        <v>341</v>
+        <v>408</v>
       </c>
       <c r="E96" t="s">
-        <v>342</v>
+        <v>12</v>
       </c>
       <c r="F96" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="G96" t="s">
         <v>18</v>
       </c>
       <c r="H96" t="s">
         <v>19</v>
-      </c>
-      <c r="I96" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>344</v>
+        <v>409</v>
       </c>
       <c r="B97" t="s">
         <v>8</v>
@@ -4415,10 +4382,10 @@
         <v>16</v>
       </c>
       <c r="D97" t="s">
-        <v>345</v>
+        <v>410</v>
       </c>
       <c r="E97" t="s">
-        <v>288</v>
+        <v>12</v>
       </c>
       <c r="F97" t="s">
         <v>12</v>
@@ -4428,14 +4395,11 @@
       </c>
       <c r="H97" t="s">
         <v>19</v>
-      </c>
-      <c r="I97" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>347</v>
+        <v>49</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
@@ -4444,13 +4408,13 @@
         <v>16</v>
       </c>
       <c r="D98" t="s">
-        <v>348</v>
+        <v>50</v>
       </c>
       <c r="E98" t="s">
-        <v>349</v>
+        <v>12</v>
       </c>
       <c r="F98" t="s">
-        <v>224</v>
+        <v>12</v>
       </c>
       <c r="G98" t="s">
         <v>18</v>
@@ -4459,24 +4423,24 @@
         <v>19</v>
       </c>
       <c r="I98" t="s">
-        <v>350</v>
+        <v>51</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>351</v>
+        <v>31</v>
       </c>
       <c r="B99" t="s">
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>16</v>
+        <v>279</v>
       </c>
       <c r="D99" t="s">
-        <v>352</v>
+        <v>404</v>
       </c>
       <c r="E99" t="s">
-        <v>135</v>
+        <v>405</v>
       </c>
       <c r="F99" t="s">
         <v>12</v>
@@ -4485,114 +4449,108 @@
         <v>18</v>
       </c>
       <c r="H99" t="s">
-        <v>19</v>
+        <v>283</v>
       </c>
       <c r="I99" t="s">
-        <v>353</v>
+        <v>406</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>354</v>
+        <v>201</v>
       </c>
       <c r="B100" t="s">
         <v>8</v>
       </c>
       <c r="C100" t="s">
-        <v>16</v>
+        <v>279</v>
       </c>
       <c r="D100" t="s">
-        <v>355</v>
+        <v>280</v>
       </c>
       <c r="E100" t="s">
-        <v>91</v>
+        <v>281</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>282</v>
       </c>
       <c r="G100" t="s">
         <v>18</v>
       </c>
       <c r="H100" t="s">
-        <v>19</v>
+        <v>283</v>
       </c>
       <c r="I100" t="s">
-        <v>356</v>
+        <v>284</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>357</v>
+        <v>217</v>
       </c>
       <c r="B101" t="s">
         <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>16</v>
+        <v>218</v>
       </c>
       <c r="D101" t="s">
-        <v>358</v>
+        <v>219</v>
       </c>
       <c r="E101" t="s">
-        <v>359</v>
+        <v>12</v>
       </c>
       <c r="F101" t="s">
         <v>12</v>
       </c>
       <c r="G101" t="s">
-        <v>18</v>
+        <v>218</v>
       </c>
       <c r="H101" t="s">
-        <v>19</v>
-      </c>
-      <c r="I101" t="s">
-        <v>360</v>
+        <v>220</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>361</v>
+        <v>221</v>
       </c>
       <c r="B102" t="s">
         <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>16</v>
+        <v>222</v>
       </c>
       <c r="D102" t="s">
-        <v>362</v>
+        <v>223</v>
       </c>
       <c r="E102" t="s">
-        <v>363</v>
+        <v>12</v>
       </c>
       <c r="F102" t="s">
         <v>12</v>
       </c>
       <c r="G102" t="s">
-        <v>18</v>
+        <v>224</v>
       </c>
       <c r="H102" t="s">
-        <v>19</v>
-      </c>
-      <c r="I102" t="s">
-        <v>364</v>
+        <v>225</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>365</v>
+        <v>194</v>
       </c>
       <c r="B103" t="s">
         <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D103" t="s">
-        <v>366</v>
+        <v>195</v>
       </c>
       <c r="E103" t="s">
-        <v>367</v>
+        <v>12</v>
       </c>
       <c r="F103" t="s">
         <v>12</v>
@@ -4601,21 +4559,21 @@
         <v>18</v>
       </c>
       <c r="H103" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>368</v>
+        <v>194</v>
       </c>
       <c r="B104" t="s">
         <v>8</v>
       </c>
       <c r="C104" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D104" t="s">
-        <v>369</v>
+        <v>195</v>
       </c>
       <c r="E104" t="s">
         <v>12</v>
@@ -4627,24 +4585,27 @@
         <v>18</v>
       </c>
       <c r="H104" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+      <c r="I104" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>370</v>
+        <v>285</v>
       </c>
       <c r="B105" t="s">
         <v>8</v>
       </c>
       <c r="C105" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D105" t="s">
-        <v>371</v>
+        <v>286</v>
       </c>
       <c r="E105" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F105" t="s">
         <v>12</v>
@@ -4653,53 +4614,56 @@
         <v>18</v>
       </c>
       <c r="H105" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+      <c r="I105" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>372</v>
+        <v>41</v>
       </c>
       <c r="B106" t="s">
         <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D106" t="s">
-        <v>373</v>
+        <v>43</v>
       </c>
       <c r="E106" t="s">
-        <v>374</v>
+        <v>44</v>
       </c>
       <c r="F106" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="G106" t="s">
         <v>18</v>
       </c>
       <c r="H106" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="I106" t="s">
-        <v>375</v>
+        <v>419</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>202</v>
+        <v>46</v>
       </c>
       <c r="B107" t="s">
         <v>8</v>
       </c>
       <c r="C107" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D107" t="s">
-        <v>376</v>
+        <v>47</v>
       </c>
       <c r="E107" t="s">
-        <v>377</v>
+        <v>291</v>
       </c>
       <c r="F107" t="s">
         <v>12</v>
@@ -4708,27 +4672,27 @@
         <v>18</v>
       </c>
       <c r="H107" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="I107" t="s">
-        <v>378</v>
+        <v>48</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>379</v>
+        <v>287</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
       </c>
       <c r="C108" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D108" t="s">
-        <v>380</v>
+        <v>288</v>
       </c>
       <c r="E108" t="s">
-        <v>381</v>
+        <v>420</v>
       </c>
       <c r="F108" t="s">
         <v>12</v>
@@ -4737,27 +4701,27 @@
         <v>18</v>
       </c>
       <c r="H108" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="I108" t="s">
-        <v>382</v>
+        <v>421</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>383</v>
+        <v>289</v>
       </c>
       <c r="B109" t="s">
         <v>8</v>
       </c>
       <c r="C109" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D109" t="s">
-        <v>384</v>
+        <v>290</v>
       </c>
       <c r="E109" t="s">
-        <v>161</v>
+        <v>291</v>
       </c>
       <c r="F109" t="s">
         <v>12</v>
@@ -4766,389 +4730,398 @@
         <v>18</v>
       </c>
       <c r="H109" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="I109" t="s">
-        <v>385</v>
+        <v>292</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>386</v>
+        <v>197</v>
       </c>
       <c r="B110" t="s">
         <v>8</v>
       </c>
       <c r="C110" t="s">
-        <v>16</v>
+        <v>198</v>
       </c>
       <c r="D110" t="s">
-        <v>387</v>
+        <v>199</v>
       </c>
       <c r="E110" t="s">
-        <v>97</v>
+        <v>200</v>
       </c>
       <c r="F110" t="s">
-        <v>12</v>
+        <v>201</v>
       </c>
       <c r="G110" t="s">
         <v>18</v>
       </c>
       <c r="H110" t="s">
-        <v>19</v>
+        <v>202</v>
       </c>
       <c r="I110" t="s">
-        <v>388</v>
+        <v>203</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>389</v>
+        <v>204</v>
       </c>
       <c r="B111" t="s">
         <v>8</v>
       </c>
       <c r="C111" t="s">
-        <v>16</v>
+        <v>198</v>
       </c>
       <c r="D111" t="s">
-        <v>390</v>
+        <v>205</v>
       </c>
       <c r="E111" t="s">
-        <v>363</v>
+        <v>422</v>
       </c>
       <c r="F111" t="s">
-        <v>12</v>
+        <v>206</v>
       </c>
       <c r="G111" t="s">
         <v>18</v>
       </c>
       <c r="H111" t="s">
-        <v>19</v>
+        <v>202</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>391</v>
+        <v>293</v>
       </c>
       <c r="B112" t="s">
         <v>8</v>
       </c>
       <c r="C112" t="s">
-        <v>16</v>
+        <v>198</v>
       </c>
       <c r="D112" t="s">
-        <v>392</v>
+        <v>294</v>
       </c>
       <c r="E112" t="s">
-        <v>393</v>
+        <v>423</v>
       </c>
       <c r="F112" t="s">
-        <v>12</v>
+        <v>295</v>
       </c>
       <c r="G112" t="s">
         <v>18</v>
       </c>
       <c r="H112" t="s">
-        <v>19</v>
+        <v>202</v>
       </c>
       <c r="I112" t="s">
-        <v>394</v>
+        <v>424</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>395</v>
+        <v>296</v>
       </c>
       <c r="B113" t="s">
         <v>8</v>
       </c>
       <c r="C113" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D113" t="s">
-        <v>396</v>
+        <v>297</v>
       </c>
       <c r="E113" t="s">
-        <v>397</v>
+        <v>55</v>
       </c>
       <c r="F113" t="s">
-        <v>12</v>
+        <v>298</v>
       </c>
       <c r="G113" t="s">
         <v>18</v>
       </c>
       <c r="H113" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="I113" t="s">
-        <v>398</v>
+        <v>299</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>175</v>
+        <v>300</v>
       </c>
       <c r="B114" t="s">
         <v>8</v>
       </c>
       <c r="C114" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D114" t="s">
-        <v>399</v>
+        <v>301</v>
       </c>
       <c r="E114" t="s">
-        <v>400</v>
+        <v>302</v>
       </c>
       <c r="F114" t="s">
-        <v>12</v>
+        <v>303</v>
       </c>
       <c r="G114" t="s">
         <v>18</v>
       </c>
       <c r="H114" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="I114" t="s">
-        <v>401</v>
+        <v>304</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>402</v>
+        <v>52</v>
       </c>
       <c r="B115" t="s">
         <v>8</v>
       </c>
       <c r="C115" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D115" t="s">
-        <v>403</v>
+        <v>54</v>
       </c>
       <c r="E115" t="s">
-        <v>404</v>
+        <v>55</v>
       </c>
       <c r="F115" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="G115" t="s">
         <v>18</v>
       </c>
       <c r="H115" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="I115" t="s">
-        <v>405</v>
+        <v>58</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>406</v>
+        <v>305</v>
       </c>
       <c r="B116" t="s">
         <v>8</v>
       </c>
       <c r="C116" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D116" t="s">
-        <v>407</v>
+        <v>306</v>
       </c>
       <c r="E116" t="s">
-        <v>408</v>
+        <v>307</v>
       </c>
       <c r="F116" t="s">
-        <v>402</v>
+        <v>65</v>
       </c>
       <c r="G116" t="s">
         <v>18</v>
       </c>
       <c r="H116" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="I116" t="s">
-        <v>409</v>
+        <v>308</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>186</v>
+        <v>309</v>
       </c>
       <c r="B117" t="s">
         <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D117" t="s">
-        <v>410</v>
+        <v>310</v>
       </c>
       <c r="E117" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="F117" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="G117" t="s">
         <v>18</v>
       </c>
       <c r="H117" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="I117" t="s">
-        <v>411</v>
+        <v>311</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>412</v>
+        <v>59</v>
       </c>
       <c r="B118" t="s">
         <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D118" t="s">
-        <v>413</v>
+        <v>60</v>
       </c>
       <c r="E118" t="s">
-        <v>182</v>
+        <v>61</v>
       </c>
       <c r="F118" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G118" t="s">
         <v>18</v>
       </c>
       <c r="H118" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="I118" t="s">
-        <v>183</v>
+        <v>425</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>414</v>
+        <v>312</v>
       </c>
       <c r="B119" t="s">
         <v>8</v>
       </c>
       <c r="C119" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D119" t="s">
-        <v>415</v>
+        <v>313</v>
       </c>
       <c r="E119" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="F119" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="G119" t="s">
         <v>18</v>
       </c>
       <c r="H119" t="s">
-        <v>19</v>
+        <v>57</v>
+      </c>
+      <c r="I119" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>416</v>
+        <v>62</v>
       </c>
       <c r="B120" t="s">
         <v>8</v>
       </c>
       <c r="C120" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D120" t="s">
-        <v>417</v>
+        <v>63</v>
       </c>
       <c r="E120" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="F120" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="G120" t="s">
         <v>18</v>
       </c>
       <c r="H120" t="s">
-        <v>19</v>
+        <v>57</v>
+      </c>
+      <c r="I120" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>418</v>
+        <v>212</v>
       </c>
       <c r="B121" t="s">
         <v>8</v>
       </c>
       <c r="C121" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D121" t="s">
-        <v>419</v>
+        <v>213</v>
       </c>
       <c r="E121" t="s">
-        <v>12</v>
+        <v>214</v>
       </c>
       <c r="F121" t="s">
-        <v>12</v>
+        <v>215</v>
       </c>
       <c r="G121" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H121" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="I121" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>420</v>
+        <v>7</v>
       </c>
       <c r="B122" t="s">
         <v>8</v>
       </c>
       <c r="C122" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D122" t="s">
-        <v>421</v>
+        <v>10</v>
       </c>
       <c r="E122" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F122" t="s">
         <v>12</v>
       </c>
       <c r="G122" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H122" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>422</v>
+        <v>207</v>
       </c>
       <c r="B123" t="s">
         <v>8</v>
       </c>
       <c r="C123" t="s">
-        <v>16</v>
+        <v>208</v>
       </c>
       <c r="D123" t="s">
-        <v>423</v>
+        <v>209</v>
       </c>
       <c r="E123" t="s">
-        <v>12</v>
+        <v>194</v>
       </c>
       <c r="F123" t="s">
         <v>12</v>
@@ -5157,12 +5130,15 @@
         <v>18</v>
       </c>
       <c r="H123" t="s">
-        <v>19</v>
+        <v>210</v>
+      </c>
+      <c r="I123" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
       <c r="B124" t="s">
         <v>8</v>
@@ -5171,7 +5147,7 @@
         <v>16</v>
       </c>
       <c r="D124" t="s">
-        <v>425</v>
+        <v>403</v>
       </c>
       <c r="E124" t="s">
         <v>12</v>
@@ -5188,19 +5164,19 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B125" t="s">
         <v>8</v>
       </c>
       <c r="C125" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="D125" t="s">
-        <v>426</v>
+        <v>404</v>
       </c>
       <c r="E125" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="F125" t="s">
         <v>12</v>
@@ -5209,15 +5185,15 @@
         <v>18</v>
       </c>
       <c r="H125" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="I125" t="s">
-        <v>428</v>
+        <v>406</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>429</v>
+        <v>407</v>
       </c>
       <c r="B126" t="s">
         <v>8</v>
@@ -5226,7 +5202,7 @@
         <v>16</v>
       </c>
       <c r="D126" t="s">
-        <v>430</v>
+        <v>408</v>
       </c>
       <c r="E126" t="s">
         <v>12</v>
@@ -5243,7 +5219,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>431</v>
+        <v>409</v>
       </c>
       <c r="B127" t="s">
         <v>8</v>
@@ -5252,7 +5228,7 @@
         <v>16</v>
       </c>
       <c r="D127" t="s">
-        <v>432</v>
+        <v>410</v>
       </c>
       <c r="E127" t="s">
         <v>12</v>
@@ -5268,6 +5244,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I127" xr:uid="{FC80CAC8-273C-4A06-BC59-43F7C812F734}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>